<commit_message>
Revised OneOnOne specific design file.
</commit_message>
<xml_diff>
--- a/skrum_docs/04_SpecificDesign/41_OneOnOne_20171017.xlsx
+++ b/skrum_docs/04_SpecificDesign/41_OneOnOne_20171017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="460" windowWidth="27700" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="-25600" yWindow="0" windowWidth="25600" windowHeight="20480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="目標管理画面" sheetId="1" r:id="rId1"/>
@@ -6669,132 +6669,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="四角形吹き出し 5"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10363200" y="177800"/>
-          <a:ext cx="838200" cy="444500"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 26293"/>
-            <a:gd name="adj2" fmla="val 83204"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
-            <a:t>sdate</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="四角形吹き出し 6"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11595100" y="139700"/>
-          <a:ext cx="838200" cy="444500"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 6596"/>
-            <a:gd name="adj2" fmla="val 91775"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
-            <a:t>edate</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -9492,7 +9366,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>フィードバック種類：</a:t>
+            <a:t>フィードバック種別：</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -10642,6 +10516,323 @@
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>889000</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="67" name="図 66"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2501900" y="19278600"/>
+          <a:ext cx="647700" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>241300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="図 67"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1955800" y="19265900"/>
+          <a:ext cx="508000" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="強調線吹き出し 2 (枠付き) 68"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13779500" y="292100"/>
+          <a:ext cx="3479800" cy="1320800"/>
+        </a:xfrm>
+        <a:prstGeom prst="accentBorderCallout2">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 18750"/>
+            <a:gd name="adj2" fmla="val -8333"/>
+            <a:gd name="adj3" fmla="val 11932"/>
+            <a:gd name="adj4" fmla="val -311475"/>
+            <a:gd name="adj5" fmla="val 43668"/>
+            <a:gd name="adj6" fmla="val -321697"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Right order.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>日報</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>進捗メモ</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ヒアリング</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>フィードバック</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>面談メモ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="四角形吹き出し 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10363200" y="177800"/>
+          <a:ext cx="838200" cy="444500"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 26293"/>
+            <a:gd name="adj2" fmla="val 83204"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
+            <a:t>sdate</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="四角形吹き出し 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11595100" y="139700"/>
+          <a:ext cx="838200" cy="444500"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 6596"/>
+            <a:gd name="adj2" fmla="val 91775"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
+            <a:t>edate</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>

</xml_diff>

<commit_message>
AP0105 - Added unreadFlgCounts.
</commit_message>
<xml_diff>
--- a/skrum_docs/04_SpecificDesign/41_OneOnOne_20171017.xlsx
+++ b/skrum_docs/04_SpecificDesign/41_OneOnOne_20171017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="0" windowWidth="25600" windowHeight="20480" tabRatio="500"/>
+    <workbookView xWindow="1100" yWindow="460" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="目標管理画面" sheetId="1" r:id="rId1"/>
@@ -4090,7 +4090,15 @@
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="mr-IN" altLang="ja-JP" sz="1800"/>
-            <a:t>"oneOnOneType": "4",</a:t>
+            <a:t>"oneOnOneType": "</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
+            <a:t>3</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="mr-IN" altLang="ja-JP" sz="1800"/>
+            <a:t>",</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
         </a:p>
@@ -4314,7 +4322,15 @@
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="mr-IN" altLang="ja-JP" sz="1800"/>
-            <a:t>"oneOnOneType": "4",</a:t>
+            <a:t>"oneOnOneType": "</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
+            <a:t>3</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="mr-IN" altLang="ja-JP" sz="1800"/>
+            <a:t>",</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
         </a:p>
@@ -4702,7 +4718,15 @@
           </a:pPr>
           <a:r>
             <a:rPr kumimoji="1" lang="mr-IN" altLang="ja-JP" sz="1800"/>
-            <a:t>{  "oneOnOneType": "3",</a:t>
+            <a:t>{  "oneOnOneType": "</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
+            <a:t>4</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="mr-IN" altLang="ja-JP" sz="1800"/>
+            <a:t>",</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
         </a:p>
@@ -4926,7 +4950,15 @@
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="mr-IN" altLang="ja-JP" sz="1800"/>
-            <a:t>"oneOnOneType": "3",</a:t>
+            <a:t>"oneOnOneType": "</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
+            <a:t>4</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="mr-IN" altLang="ja-JP" sz="1800"/>
+            <a:t>",</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
         </a:p>
@@ -6143,7 +6175,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
-            <a:t>/users/{userId}/defaultdestinations.json&amp;oootype=4</a:t>
+            <a:t>/users/{userId}/defaultdestinations.json&amp;oootype=3</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6221,7 +6253,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
-            <a:t>/users/{userId}/defaultdestinations.json&amp;oootype=3</a:t>
+            <a:t>/users/{userId}/defaultdestinations.json&amp;oootype=4</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6849,7 +6881,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
-            <a:t>oootype="4"</a:t>
+            <a:t>oootype="3"</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6912,7 +6944,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
-            <a:t>oootype="3"</a:t>
+            <a:t>oootype="4"</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>

</xml_diff>